<commit_message>
Added groups and xml groups
</commit_message>
<xml_diff>
--- a/test_data_sauce_demo.xlsx
+++ b/test_data_sauce_demo.xlsx
@@ -14,22 +14,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>Shaun</t>
+    <t>Karina</t>
   </si>
   <si>
-    <t>n3c1o8pset1c</t>
+    <t>adytx1yloe96so</t>
   </si>
   <si>
-    <t>Leonel</t>
+    <t>Melony</t>
   </si>
   <si>
-    <t>ithlzlmx</t>
+    <t>ome71tlpz</t>
   </si>
   <si>
-    <t>Glenna</t>
+    <t>Dawn</t>
   </si>
   <si>
-    <t>9hsic5tbsveb5l4</t>
+    <t>5qcrnbwc7</t>
   </si>
 </sst>
 </file>

</xml_diff>